<commit_message>
Updating Excel template and HEVApp
</commit_message>
<xml_diff>
--- a/src/HEVDoc.xlsx
+++ b/src/HEVDoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcarniel\MATLAB Drive\Demo\HEVProject\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcarniel\MATLAB Drive\Demo\hev-p4-app\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E0520D-89A8-43C5-BCF5-447A8FB1EECC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A764A7F-E016-4E2D-88C1-DA274D0408C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A1885300-66AE-41D9-AAA4-7C47AF3BCC37}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1885300-66AE-41D9-AAA4-7C47AF3BCC37}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -55,23 +55,23 @@
     <t>By default, the HEV P4 reference application is configured with:</t>
   </si>
   <si>
-    <t xml:space="preserve">The hybrid electric vehicle (HEV) P4 reference application represents a full HEV model with an internal combustion engine, transmission, battery, motor, and associated powertrain control algorithms. Use the reference application for hardware-in-the-loop (HIL) testing, tradeoff analysis, and control parameter optimization of a HEV P4 hybrid. </t>
-  </si>
-  <si>
-    <t>MATLAB
-Simulink
-Powertrain Blockset
-MATLAB Report Generator
-Simulink Compiler
-MATLAB Compiler
-MATLAB Web App Server</t>
-  </si>
-  <si>
     <t xml:space="preserve">The report summarizes the results of a fleet test campaign of the hybrid electric vehicle (HEV) P4 model. The document provides both the model setup info and results.
 </t>
   </si>
   <si>
-    <t>MATLAB R2021a</t>
+    <t>MATLAB®
+Simulink®
+Powertrain Blockset™
+MATLAB® Report Generator™
+Simulink® Compiler™
+MATLAB® Compiler™
+MATLAB® Web App Server™</t>
+  </si>
+  <si>
+    <t>MATLAB® R2021a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Hybrid Electric Vehicle (HEV) P4 Reference Application represents a full HEV model with an internal combustion engine, transmission, battery, motor, and associated powertrain control algorithms. Use the reference application for hardware-in-the-loop (HIL) testing, tradeoff analysis, and control parameter optimization of a HEV P4 hybrid. </t>
   </si>
 </sst>
 </file>
@@ -506,22 +506,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48696F6B-4A8C-46B4-9E20-9F255847569D}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="124.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -529,23 +529,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -553,36 +553,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
     </row>
   </sheetData>
@@ -599,267 +599,267 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
@@ -870,6 +870,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100849E6C8D9EB5C240A18821361A059B32" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d6bc2246ce23975edf22398fc6725d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1ef0d92-236c-4e1f-941d-e34880ea6a78" xmlns:ns4="564a3ec2-6573-47c4-b9f1-b3348015fabc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="acfd641fb42e00de0f8d86cd58708da7" ns3:_="" ns4:_="">
     <xsd:import namespace="a1ef0d92-236c-4e1f-941d-e34880ea6a78"/>
@@ -1092,36 +1107,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C4E11-BB67-4BB2-8EBE-EA56AEAA90ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B901FFE5-3246-4AB4-B2E2-F27BFBED62F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1ef0d92-236c-4e1f-941d-e34880ea6a78"/>
-    <ds:schemaRef ds:uri="564a3ec2-6573-47c4-b9f1-b3348015fabc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1144,9 +1133,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B901FFE5-3246-4AB4-B2E2-F27BFBED62F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C4E11-BB67-4BB2-8EBE-EA56AEAA90ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1ef0d92-236c-4e1f-941d-e34880ea6a78"/>
+    <ds:schemaRef ds:uri="564a3ec2-6573-47c4-b9f1-b3348015fabc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Big changes! Code re-written completely using OOP.
</commit_message>
<xml_diff>
--- a/src/HEVDoc.xlsx
+++ b/src/HEVDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcarniel\MATLAB Drive\Demo\hev-p4-app\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A764A7F-E016-4E2D-88C1-DA274D0408C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6200207C-33E8-4123-B0EA-1A52BDCEBA5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1885300-66AE-41D9-AAA4-7C47AF3BCC37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{A1885300-66AE-41D9-AAA4-7C47AF3BCC37}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <t>MATLAB® R2021a</t>
   </si>
   <si>
-    <t xml:space="preserve">The Hybrid Electric Vehicle (HEV) P4 Reference Application represents a full HEV model with an internal combustion engine, transmission, battery, motor, and associated powertrain control algorithms. Use the reference application for hardware-in-the-loop (HIL) testing, tradeoff analysis, and control parameter optimization of a HEV P4 hybrid. </t>
+    <t xml:space="preserve">The Hybrid Electric Vehicle (HEV) P4 Reference Application represents a full HEV model with an internal combustion engine, transmission, battery, motor, and associated powertrain control algorithms. Use the reference application for hardware-in-the-loop (HIL) testing, tradeoff analysis, and control parameter optimization of a HEV P4. </t>
   </si>
 </sst>
 </file>
@@ -507,21 +507,21 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="124.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="1"/>
+    <col min="4" max="4" width="20.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -537,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -553,7 +553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -561,28 +561,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" s="8"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
     </row>
   </sheetData>
@@ -599,267 +599,267 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="6"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="6"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="6"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="6"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="6"/>
@@ -870,21 +870,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100849E6C8D9EB5C240A18821361A059B32" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d6bc2246ce23975edf22398fc6725d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1ef0d92-236c-4e1f-941d-e34880ea6a78" xmlns:ns4="564a3ec2-6573-47c4-b9f1-b3348015fabc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="acfd641fb42e00de0f8d86cd58708da7" ns3:_="" ns4:_="">
     <xsd:import namespace="a1ef0d92-236c-4e1f-941d-e34880ea6a78"/>
@@ -1107,10 +1092,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B901FFE5-3246-4AB4-B2E2-F27BFBED62F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C4E11-BB67-4BB2-8EBE-EA56AEAA90ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1ef0d92-236c-4e1f-941d-e34880ea6a78"/>
+    <ds:schemaRef ds:uri="564a3ec2-6573-47c4-b9f1-b3348015fabc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1133,20 +1144,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C4E11-BB67-4BB2-8EBE-EA56AEAA90ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B901FFE5-3246-4AB4-B2E2-F27BFBED62F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1ef0d92-236c-4e1f-941d-e34880ea6a78"/>
-    <ds:schemaRef ds:uri="564a3ec2-6573-47c4-b9f1-b3348015fabc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>